<commit_message>
create main GUI and some controllers
</commit_message>
<xml_diff>
--- a/datafiles/club.xlsx
+++ b/datafiles/club.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="90" windowWidth="19200" windowHeight="11640"/>
@@ -11,13 +11,57 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="125725"/>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+  <si>
+    <t>Club name</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Home stadium</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Coach</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ranking</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Real Madrid</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Liverpool</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Brendan Rodgers</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Anfield</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Santiago Bernabeu</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Carlo Ancelotti</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -32,6 +76,17 @@
       <family val="2"/>
       <charset val="134"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -56,9 +111,15 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -354,12 +415,66 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1"/>
+  <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="16.125" customWidth="1"/>
+    <col min="2" max="2" width="18.25" customWidth="1"/>
+    <col min="3" max="3" width="19.75" customWidth="1"/>
+    <col min="4" max="4" width="11.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" ht="14.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5" ht="14.25">
+      <c r="A2" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="D2" s="1">
+        <v>1</v>
+      </c>
+      <c r="E2" s="1"/>
+    </row>
+    <row r="3" spans="1:5" ht="14.25">
+      <c r="A3" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3" s="1">
+        <v>43</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+  </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200" r:id="rId1"/>

</xml_diff>